<commit_message>
Change RestApi list name
</commit_message>
<xml_diff>
--- a/프로젝트 API 문서/RestAPI List.xlsx
+++ b/프로젝트 API 문서/RestAPI List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeong-gyeongjae/Desktop/Graduations/Security-docs/프로젝트 API 문서/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E35439-123A-D24D-9940-00318D1375A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32747BB3-2288-F441-88A4-D4F135814EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{E694652C-9148-3840-A4B3-A701D42115EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>메인페이지(로그인전)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,6 +235,10 @@
   </si>
   <si>
     <t>추후 다른단어 교체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/users/login/oauth2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1454,7 +1458,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
@@ -1532,6 +1536,9 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">

</xml_diff>

<commit_message>
Fix APIList and Back-end 개발현황
</commit_message>
<xml_diff>
--- a/프로젝트 API 문서/RestAPI List.xlsx
+++ b/프로젝트 API 문서/RestAPI List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeong-gyeongjae/Desktop/Graduations/Security-docs/프로젝트 API 문서/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B4E4CD-4FB6-E74F-967C-5E2C21C7E6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE3A5C9-0B01-B946-AE7E-DE955CB518AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{E694652C-9148-3840-A4B3-A701D42115EA}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{E694652C-9148-3840-A4B3-A701D42115EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31ECD4EB-599C-534A-A0BB-8DBE5A2E2D56}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>

</xml_diff>

<commit_message>
Fix Rest API List
</commit_message>
<xml_diff>
--- a/프로젝트 API 문서/RestAPI List.xlsx
+++ b/프로젝트 API 문서/RestAPI List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeong-gyeongjae/Desktop/Graduations/Security-docs/프로젝트 API 문서/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE3A5C9-0B01-B946-AE7E-DE955CB518AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863DA15E-D9FF-EF49-855B-17D139F8D7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{E694652C-9148-3840-A4B3-A701D42115EA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{E694652C-9148-3840-A4B3-A701D42115EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -230,10 +230,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cont/securitynotices</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>계좌 생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,6 +247,10 @@
   </si>
   <si>
     <t>/users/accounts/transaction/success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cont/security-notices</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
@@ -1617,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -1649,10 +1649,10 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
         <v>49</v>
-      </c>
-      <c r="D24" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -1660,7 +1660,7 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:5">
@@ -1668,7 +1668,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -1676,7 +1676,7 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:5">

</xml_diff>